<commit_message>
update otp input example
</commit_message>
<xml_diff>
--- a/examples/input/otp.xlsx
+++ b/examples/input/otp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoltantudlik/Development/ynab-csv-converter/examples/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73A114B-3F33-E44A-BBE9-654034A41F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE20E954-3E61-684F-AFFA-E86BB1A64121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Tranzakció dátuma</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>09. HAVI MUNKABER</t>
+  </si>
+  <si>
+    <t>21029112-11111112-25163151</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -591,8 +594,8 @@
       <c r="E2" t="s">
         <v>41</v>
       </c>
-      <c r="F2">
-        <v>1.0818001000000001E+23</v>
+      <c r="F2" t="s">
+        <v>43</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
@@ -705,8 +708,8 @@
       <c r="E5" t="s">
         <v>34</v>
       </c>
-      <c r="F5">
-        <v>2288449514267340</v>
+      <c r="F5" t="s">
+        <v>43</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>

</xml_diff>